<commit_message>
fix generic class loop
</commit_message>
<xml_diff>
--- a/bases/output_V5.xlsx
+++ b/bases/output_V5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Levenshtein-Distance\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8264DC-3189-4753-9F0C-D9EA1BF81F2B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5E2F3C-33D1-4096-AB1B-EB68EF0FDB7F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -279,7 +279,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +289,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -329,6 +335,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,13 +643,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="83" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
@@ -1128,35 +1138,35 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>323</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <v>96</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16">
-        <v>29094658</v>
-      </c>
-      <c r="H16">
-        <v>29094658</v>
-      </c>
-      <c r="I16">
+      <c r="F16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="5">
+        <v>29094658</v>
+      </c>
+      <c r="H16" s="5">
+        <v>29094658</v>
+      </c>
+      <c r="I16" s="5">
         <v>14</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="5">
         <v>1569</v>
       </c>
     </row>
@@ -1801,7 +1811,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B36" xr:uid="{1DC2BEE1-4DFA-49BB-A032-6E59D2357363}"/>
+  <autoFilter ref="A1:J1" xr:uid="{B3F5A559-E9EC-4158-A9CD-892E89942F0A}"/>
   <sortState ref="A2:J36">
     <sortCondition ref="B1"/>
   </sortState>

</xml_diff>